<commit_message>
ID 5277764602 - Total Weight
Added a SumProduct formula to the "Total Weight" cell to automatically multiply the unit weight with the quantity of each item.
</commit_message>
<xml_diff>
--- a/02_Beta/IWR V1.8.xlsx
+++ b/02_Beta/IWR V1.8.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\Shared\Z_DevCyntech\KZS\06_IWR\00_GM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A DEV\kzs-tkt-2106-IWR\02_Beta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3588F63-967B-4F3C-A3B2-B1B0337CDD6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FED9463-C1BC-479E-80D9-CC21533BC26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -484,13 +484,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="7">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
-    <numFmt numFmtId="166" formatCode="00000"/>
-    <numFmt numFmtId="167" formatCode="#,##0&quot; lbs&quot;"/>
-    <numFmt numFmtId="168" formatCode="#,##0&quot; hrs&quot;"/>
-    <numFmt numFmtId="169" formatCode="0."/>
-    <numFmt numFmtId="170" formatCode="#,##0.0&quot; wks&quot;"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
+    <numFmt numFmtId="166" formatCode="#,##0&quot; lbs&quot;"/>
+    <numFmt numFmtId="167" formatCode="#,##0&quot; hrs&quot;"/>
+    <numFmt numFmtId="168" formatCode="0."/>
+    <numFmt numFmtId="169" formatCode="#,##0.0&quot; wks&quot;"/>
   </numFmts>
   <fonts count="24" x14ac:knownFonts="1">
     <font>
@@ -1039,7 +1039,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1116,7 +1116,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
@@ -1136,6 +1136,130 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="169" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="167" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1146,6 +1270,174 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="top" indent="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="3" fontId="4" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
       <protection locked="0"/>
@@ -1153,298 +1445,6 @@
     <xf numFmtId="3" fontId="4" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top" indent="1"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="2" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="4" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="top" indent="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="20" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="170" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="167" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="2" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1849,7 +1849,7 @@
   <dimension ref="A1:AF339"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+      <selection activeCell="P13" sqref="P13:Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1890,11 +1890,11 @@
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="58"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="58"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
@@ -1902,21 +1902,21 @@
     </row>
     <row r="2" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="59"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="65"/>
+      <c r="I2" s="65"/>
+      <c r="J2" s="65"/>
+      <c r="K2" s="65"/>
+      <c r="L2" s="65"/>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
     </row>
@@ -1945,19 +1945,19 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="G4" s="95"/>
-      <c r="H4" s="95"/>
-      <c r="I4" s="95"/>
-      <c r="J4" s="95"/>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="85" t="s">
+      <c r="N4" s="28" t="s">
         <v>57</v>
       </c>
-      <c r="O4" s="91"/>
-      <c r="P4" s="91"/>
-      <c r="Q4" s="92"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30"/>
+      <c r="Q4" s="31"/>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1968,17 +1968,17 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="G5" s="95"/>
-      <c r="H5" s="95"/>
-      <c r="I5" s="95"/>
-      <c r="J5" s="95"/>
-      <c r="K5" s="95"/>
-      <c r="L5" s="95"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="87"/>
-      <c r="O5" s="93"/>
-      <c r="P5" s="93"/>
-      <c r="Q5" s="94"/>
+      <c r="N5" s="29"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="32"/>
+      <c r="Q5" s="33"/>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1989,12 +1989,12 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="G6" s="96"/>
-      <c r="H6" s="96"/>
-      <c r="I6" s="96"/>
-      <c r="J6" s="96"/>
-      <c r="K6" s="96"/>
-      <c r="L6" s="96"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
       <c r="M6" s="1"/>
       <c r="R6" s="1"/>
     </row>
@@ -2006,24 +2006,24 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="G7" s="96" t="s">
+      <c r="G7" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="H7" s="96"/>
-      <c r="I7" s="96"/>
-      <c r="J7" s="96"/>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="35"/>
+      <c r="L7" s="35"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="85" t="s">
+      <c r="N7" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="86"/>
-      <c r="P7" s="91">
+      <c r="O7" s="40"/>
+      <c r="P7" s="30">
         <f>ROUND((G13-G11)/7,1)</f>
         <v>0</v>
       </c>
-      <c r="Q7" s="92"/>
+      <c r="Q7" s="31"/>
       <c r="R7" s="1"/>
     </row>
     <row r="8" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2034,17 +2034,17 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="G8" s="96"/>
-      <c r="H8" s="96"/>
-      <c r="I8" s="96"/>
-      <c r="J8" s="96"/>
-      <c r="K8" s="96"/>
-      <c r="L8" s="96"/>
+      <c r="G8" s="35"/>
+      <c r="H8" s="35"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="35"/>
+      <c r="L8" s="35"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="87"/>
-      <c r="O8" s="88"/>
-      <c r="P8" s="93"/>
-      <c r="Q8" s="94"/>
+      <c r="N8" s="29"/>
+      <c r="O8" s="41"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="33"/>
       <c r="R8" s="1"/>
     </row>
     <row r="9" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2082,14 +2082,14 @@
       <c r="K10" s="13"/>
       <c r="L10" s="13"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="85" t="s">
+      <c r="N10" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="O10" s="86"/>
-      <c r="P10" s="101">
+      <c r="O10" s="40"/>
+      <c r="P10" s="42">
         <v>0</v>
       </c>
-      <c r="Q10" s="102"/>
+      <c r="Q10" s="43"/>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2100,19 +2100,19 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
+      <c r="G11" s="95"/>
+      <c r="H11" s="95"/>
       <c r="I11"/>
-      <c r="J11" s="105" t="s">
+      <c r="J11" s="47" t="s">
         <v>59</v>
       </c>
-      <c r="K11" s="105"/>
-      <c r="L11" s="105"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="47"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="87"/>
-      <c r="O11" s="88"/>
-      <c r="P11" s="103"/>
-      <c r="Q11" s="104"/>
+      <c r="N11" s="29"/>
+      <c r="O11" s="41"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="45"/>
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2123,12 +2123,12 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
       <c r="I12"/>
-      <c r="J12" s="105"/>
-      <c r="K12" s="105"/>
-      <c r="L12" s="105"/>
+      <c r="J12" s="47"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
       <c r="M12" s="1"/>
       <c r="R12" s="1"/>
     </row>
@@ -2140,21 +2140,22 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
       <c r="I13"/>
-      <c r="J13" s="105"/>
-      <c r="K13" s="105"/>
-      <c r="L13" s="105"/>
+      <c r="J13" s="47"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="47"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="85" t="s">
+      <c r="N13" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="O13" s="86"/>
-      <c r="P13" s="97">
+      <c r="O13" s="40"/>
+      <c r="P13" s="36">
+        <f>SUMPRODUCT(O20:O43,C20:C43)</f>
         <v>0</v>
       </c>
-      <c r="Q13" s="98"/>
+      <c r="Q13" s="37"/>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2165,17 +2166,17 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
       <c r="I14"/>
-      <c r="J14" s="105"/>
-      <c r="K14" s="105"/>
-      <c r="L14" s="105"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
       <c r="M14" s="1"/>
-      <c r="N14" s="87"/>
-      <c r="O14" s="88"/>
-      <c r="P14" s="99"/>
-      <c r="Q14" s="100"/>
+      <c r="N14" s="29"/>
+      <c r="O14" s="41"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="39"/>
       <c r="R14" s="1"/>
     </row>
     <row r="15" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2248,132 +2249,132 @@
     </row>
     <row r="18" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="66" t="s">
+      <c r="E18" s="67"/>
+      <c r="F18" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
-      <c r="L18" s="67"/>
-      <c r="M18" s="67"/>
-      <c r="N18" s="68"/>
-      <c r="O18" s="28" t="s">
+      <c r="G18" s="79"/>
+      <c r="H18" s="79"/>
+      <c r="I18" s="79"/>
+      <c r="J18" s="79"/>
+      <c r="K18" s="79"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="79"/>
+      <c r="N18" s="80"/>
+      <c r="O18" s="60" t="s">
         <v>43</v>
       </c>
-      <c r="P18" s="42" t="s">
+      <c r="P18" s="87" t="s">
         <v>42</v>
       </c>
-      <c r="Q18" s="43"/>
+      <c r="Q18" s="88"/>
       <c r="R18" s="1"/>
       <c r="AE18"/>
       <c r="AF18"/>
     </row>
     <row r="19" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="70"/>
-      <c r="H19" s="70"/>
-      <c r="I19" s="70"/>
-      <c r="J19" s="70"/>
-      <c r="K19" s="70"/>
-      <c r="L19" s="70"/>
-      <c r="M19" s="70"/>
-      <c r="N19" s="71"/>
-      <c r="O19" s="29"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="45"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="82"/>
+      <c r="L19" s="82"/>
+      <c r="M19" s="82"/>
+      <c r="N19" s="83"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="89"/>
+      <c r="Q19" s="90"/>
       <c r="R19" s="1"/>
       <c r="AE19"/>
       <c r="AF19"/>
     </row>
     <row r="20" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
-      <c r="B20" s="53">
+      <c r="B20" s="56">
         <v>1</v>
       </c>
-      <c r="C20" s="56">
+      <c r="C20" s="58">
         <v>99</v>
       </c>
-      <c r="D20" s="64">
+      <c r="D20" s="70">
         <v>999</v>
       </c>
-      <c r="E20" s="65"/>
-      <c r="F20" s="72" t="s">
+      <c r="E20" s="71"/>
+      <c r="F20" s="84" t="s">
         <v>35</v>
       </c>
-      <c r="G20" s="73"/>
-      <c r="H20" s="73"/>
-      <c r="I20" s="73"/>
-      <c r="J20" s="73"/>
-      <c r="K20" s="73"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="73"/>
-      <c r="N20" s="74"/>
-      <c r="O20" s="30"/>
-      <c r="P20" s="81"/>
-      <c r="Q20" s="82"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
+      <c r="L20" s="85"/>
+      <c r="M20" s="85"/>
+      <c r="N20" s="86"/>
+      <c r="O20" s="104"/>
+      <c r="P20" s="91"/>
+      <c r="Q20" s="92"/>
       <c r="R20" s="1"/>
       <c r="AE20"/>
       <c r="AF20"/>
     </row>
     <row r="21" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="35"/>
-      <c r="F21" s="75" t="s">
+      <c r="B21" s="56"/>
+      <c r="C21" s="58"/>
+      <c r="D21" s="72"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="48" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="76"/>
-      <c r="H21" s="76"/>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
-      <c r="K21" s="76"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="76"/>
-      <c r="N21" s="77"/>
-      <c r="O21" s="31"/>
-      <c r="P21" s="39"/>
-      <c r="Q21" s="40"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="49"/>
+      <c r="M21" s="49"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="105"/>
+      <c r="P21" s="93"/>
+      <c r="Q21" s="94"/>
       <c r="R21" s="1"/>
       <c r="AE21"/>
       <c r="AF21"/>
     </row>
     <row r="22" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="57"/>
-      <c r="D22" s="36"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="78"/>
-      <c r="G22" s="79"/>
-      <c r="H22" s="79"/>
-      <c r="I22" s="79"/>
-      <c r="J22" s="79"/>
-      <c r="K22" s="79"/>
-      <c r="L22" s="79"/>
-      <c r="M22" s="79"/>
-      <c r="N22" s="80"/>
-      <c r="O22" s="31"/>
-      <c r="P22" s="39"/>
-      <c r="Q22" s="40"/>
+      <c r="B22" s="57"/>
+      <c r="C22" s="59"/>
+      <c r="D22" s="74"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="52"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="53"/>
+      <c r="O22" s="105"/>
+      <c r="P22" s="93"/>
+      <c r="Q22" s="94"/>
       <c r="R22" s="1"/>
       <c r="V22" s="14"/>
       <c r="W22" s="14"/>
@@ -2383,476 +2384,476 @@
     </row>
     <row r="23" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="52">
+      <c r="B23" s="62">
         <v>2</v>
       </c>
-      <c r="C23" s="55"/>
-      <c r="D23" s="32"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="76"/>
-      <c r="H23" s="76"/>
-      <c r="I23" s="76"/>
-      <c r="J23" s="76"/>
-      <c r="K23" s="76"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
-      <c r="N23" s="77"/>
-      <c r="O23" s="31"/>
-      <c r="P23" s="39"/>
-      <c r="Q23" s="40"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
+      <c r="F23" s="48"/>
+      <c r="G23" s="49"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="49"/>
+      <c r="M23" s="49"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="105"/>
+      <c r="P23" s="93"/>
+      <c r="Q23" s="94"/>
       <c r="R23" s="1"/>
       <c r="AE23"/>
       <c r="AF23"/>
     </row>
     <row r="24" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="53"/>
-      <c r="C24" s="56"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="35"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="76"/>
-      <c r="H24" s="76"/>
-      <c r="I24" s="76"/>
-      <c r="J24" s="76"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="76"/>
-      <c r="M24" s="76"/>
-      <c r="N24" s="77"/>
-      <c r="O24" s="31"/>
-      <c r="P24" s="39"/>
-      <c r="Q24" s="40"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="58"/>
+      <c r="D24" s="72"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="48"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="49"/>
+      <c r="M24" s="49"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="105"/>
+      <c r="P24" s="93"/>
+      <c r="Q24" s="94"/>
       <c r="R24" s="1"/>
       <c r="AE24"/>
       <c r="AF24"/>
     </row>
     <row r="25" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="57"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="78"/>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="79"/>
-      <c r="J25" s="79"/>
-      <c r="K25" s="79"/>
-      <c r="L25" s="79"/>
-      <c r="M25" s="79"/>
-      <c r="N25" s="80"/>
-      <c r="O25" s="31"/>
-      <c r="P25" s="39"/>
-      <c r="Q25" s="40"/>
+      <c r="B25" s="57"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="74"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="51"/>
+      <c r="G25" s="52"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="52"/>
+      <c r="K25" s="52"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="52"/>
+      <c r="N25" s="53"/>
+      <c r="O25" s="105"/>
+      <c r="P25" s="93"/>
+      <c r="Q25" s="94"/>
       <c r="R25" s="1"/>
       <c r="AE25"/>
       <c r="AF25"/>
     </row>
     <row r="26" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="52">
+      <c r="B26" s="62">
         <v>3</v>
       </c>
-      <c r="C26" s="55"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="76"/>
-      <c r="H26" s="76"/>
-      <c r="I26" s="76"/>
-      <c r="J26" s="76"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="76"/>
-      <c r="M26" s="76"/>
-      <c r="N26" s="77"/>
-      <c r="O26" s="31"/>
-      <c r="P26" s="39"/>
-      <c r="Q26" s="40"/>
+      <c r="C26" s="63"/>
+      <c r="D26" s="76"/>
+      <c r="E26" s="77"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="49"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="49"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="105"/>
+      <c r="P26" s="93"/>
+      <c r="Q26" s="94"/>
       <c r="R26" s="1"/>
       <c r="AE26"/>
       <c r="AF26"/>
     </row>
     <row r="27" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="53"/>
-      <c r="C27" s="56"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="35"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="76"/>
-      <c r="H27" s="76"/>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="76"/>
-      <c r="M27" s="76"/>
-      <c r="N27" s="77"/>
-      <c r="O27" s="31"/>
-      <c r="P27" s="39"/>
-      <c r="Q27" s="40"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="58"/>
+      <c r="D27" s="72"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="49"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="49"/>
+      <c r="M27" s="49"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="105"/>
+      <c r="P27" s="93"/>
+      <c r="Q27" s="94"/>
       <c r="R27" s="1"/>
       <c r="AE27"/>
       <c r="AF27"/>
     </row>
     <row r="28" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="57"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="78"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="79"/>
-      <c r="J28" s="79"/>
-      <c r="K28" s="79"/>
-      <c r="L28" s="79"/>
-      <c r="M28" s="79"/>
-      <c r="N28" s="80"/>
-      <c r="O28" s="31"/>
-      <c r="P28" s="39"/>
-      <c r="Q28" s="40"/>
+      <c r="B28" s="57"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="74"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="51"/>
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="52"/>
+      <c r="K28" s="52"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="52"/>
+      <c r="N28" s="53"/>
+      <c r="O28" s="105"/>
+      <c r="P28" s="93"/>
+      <c r="Q28" s="94"/>
       <c r="R28" s="1"/>
       <c r="AE28"/>
       <c r="AF28"/>
     </row>
     <row r="29" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="52">
+      <c r="B29" s="62">
         <v>4</v>
       </c>
-      <c r="C29" s="55"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="76"/>
-      <c r="I29" s="76"/>
-      <c r="J29" s="76"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="76"/>
-      <c r="M29" s="76"/>
-      <c r="N29" s="77"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="39"/>
-      <c r="Q29" s="40"/>
+      <c r="C29" s="63"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="105"/>
+      <c r="P29" s="93"/>
+      <c r="Q29" s="94"/>
       <c r="R29" s="1"/>
       <c r="AE29"/>
       <c r="AF29"/>
     </row>
     <row r="30" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="35"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="76"/>
-      <c r="M30" s="76"/>
-      <c r="N30" s="77"/>
-      <c r="O30" s="31"/>
-      <c r="P30" s="39"/>
-      <c r="Q30" s="40"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="58"/>
+      <c r="D30" s="72"/>
+      <c r="E30" s="73"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="49"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="49"/>
+      <c r="M30" s="49"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="105"/>
+      <c r="P30" s="93"/>
+      <c r="Q30" s="94"/>
       <c r="R30" s="1"/>
       <c r="AE30"/>
       <c r="AF30"/>
     </row>
     <row r="31" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="36"/>
-      <c r="E31" s="37"/>
-      <c r="F31" s="78"/>
-      <c r="G31" s="79"/>
-      <c r="H31" s="79"/>
-      <c r="I31" s="79"/>
-      <c r="J31" s="79"/>
-      <c r="K31" s="79"/>
-      <c r="L31" s="79"/>
-      <c r="M31" s="79"/>
-      <c r="N31" s="80"/>
-      <c r="O31" s="31"/>
-      <c r="P31" s="39"/>
-      <c r="Q31" s="40"/>
+      <c r="B31" s="57"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="75"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="52"/>
+      <c r="H31" s="52"/>
+      <c r="I31" s="52"/>
+      <c r="J31" s="52"/>
+      <c r="K31" s="52"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="52"/>
+      <c r="N31" s="53"/>
+      <c r="O31" s="105"/>
+      <c r="P31" s="93"/>
+      <c r="Q31" s="94"/>
       <c r="R31" s="1"/>
       <c r="AE31"/>
       <c r="AF31"/>
     </row>
     <row r="32" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
-      <c r="B32" s="52">
+      <c r="B32" s="62">
         <v>5</v>
       </c>
-      <c r="C32" s="55"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="76"/>
-      <c r="H32" s="76"/>
-      <c r="I32" s="76"/>
-      <c r="J32" s="76"/>
-      <c r="K32" s="76"/>
-      <c r="L32" s="76"/>
-      <c r="M32" s="76"/>
-      <c r="N32" s="77"/>
-      <c r="O32" s="31"/>
-      <c r="P32" s="39"/>
-      <c r="Q32" s="40"/>
+      <c r="C32" s="63"/>
+      <c r="D32" s="76"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="49"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="49"/>
+      <c r="M32" s="49"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="105"/>
+      <c r="P32" s="93"/>
+      <c r="Q32" s="94"/>
       <c r="R32" s="1"/>
       <c r="AE32"/>
       <c r="AF32"/>
     </row>
     <row r="33" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="56"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="35"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="76"/>
-      <c r="H33" s="76"/>
-      <c r="I33" s="76"/>
-      <c r="J33" s="76"/>
-      <c r="K33" s="76"/>
-      <c r="L33" s="76"/>
-      <c r="M33" s="76"/>
-      <c r="N33" s="77"/>
-      <c r="O33" s="31"/>
-      <c r="P33" s="39"/>
-      <c r="Q33" s="40"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="58"/>
+      <c r="D33" s="72"/>
+      <c r="E33" s="73"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="49"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="49"/>
+      <c r="M33" s="49"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="105"/>
+      <c r="P33" s="93"/>
+      <c r="Q33" s="94"/>
       <c r="R33" s="1"/>
       <c r="AE33"/>
       <c r="AF33"/>
     </row>
     <row r="34" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="57"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="37"/>
-      <c r="F34" s="78"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="79"/>
-      <c r="J34" s="79"/>
-      <c r="K34" s="79"/>
-      <c r="L34" s="79"/>
-      <c r="M34" s="79"/>
-      <c r="N34" s="80"/>
-      <c r="O34" s="31"/>
-      <c r="P34" s="39"/>
-      <c r="Q34" s="40"/>
+      <c r="B34" s="57"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="74"/>
+      <c r="E34" s="75"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="52"/>
+      <c r="H34" s="52"/>
+      <c r="I34" s="52"/>
+      <c r="J34" s="52"/>
+      <c r="K34" s="52"/>
+      <c r="L34" s="52"/>
+      <c r="M34" s="52"/>
+      <c r="N34" s="53"/>
+      <c r="O34" s="105"/>
+      <c r="P34" s="93"/>
+      <c r="Q34" s="94"/>
       <c r="R34" s="1"/>
       <c r="AE34"/>
       <c r="AF34"/>
     </row>
     <row r="35" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
-      <c r="B35" s="52">
+      <c r="B35" s="62">
         <v>6</v>
       </c>
-      <c r="C35" s="55"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="76"/>
-      <c r="H35" s="76"/>
-      <c r="I35" s="76"/>
-      <c r="J35" s="76"/>
-      <c r="K35" s="76"/>
-      <c r="L35" s="76"/>
-      <c r="M35" s="76"/>
-      <c r="N35" s="77"/>
-      <c r="O35" s="31"/>
-      <c r="P35" s="39"/>
-      <c r="Q35" s="40"/>
+      <c r="C35" s="63"/>
+      <c r="D35" s="76"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="48"/>
+      <c r="G35" s="49"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="49"/>
+      <c r="M35" s="49"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="105"/>
+      <c r="P35" s="93"/>
+      <c r="Q35" s="94"/>
       <c r="R35" s="1"/>
       <c r="AE35"/>
       <c r="AF35"/>
     </row>
     <row r="36" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="56"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="35"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="76"/>
-      <c r="H36" s="76"/>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="K36" s="76"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
-      <c r="N36" s="77"/>
-      <c r="O36" s="31"/>
-      <c r="P36" s="39"/>
-      <c r="Q36" s="40"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="58"/>
+      <c r="D36" s="72"/>
+      <c r="E36" s="73"/>
+      <c r="F36" s="48"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="49"/>
+      <c r="M36" s="49"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="105"/>
+      <c r="P36" s="93"/>
+      <c r="Q36" s="94"/>
       <c r="R36" s="1"/>
       <c r="AE36"/>
       <c r="AF36"/>
     </row>
     <row r="37" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="57"/>
-      <c r="D37" s="36"/>
-      <c r="E37" s="37"/>
-      <c r="F37" s="78"/>
-      <c r="G37" s="79"/>
-      <c r="H37" s="79"/>
-      <c r="I37" s="79"/>
-      <c r="J37" s="79"/>
-      <c r="K37" s="79"/>
-      <c r="L37" s="79"/>
-      <c r="M37" s="79"/>
-      <c r="N37" s="80"/>
-      <c r="O37" s="31"/>
-      <c r="P37" s="39"/>
-      <c r="Q37" s="40"/>
+      <c r="B37" s="57"/>
+      <c r="C37" s="59"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="52"/>
+      <c r="H37" s="52"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="52"/>
+      <c r="L37" s="52"/>
+      <c r="M37" s="52"/>
+      <c r="N37" s="53"/>
+      <c r="O37" s="105"/>
+      <c r="P37" s="93"/>
+      <c r="Q37" s="94"/>
       <c r="R37" s="1"/>
       <c r="AE37"/>
       <c r="AF37"/>
     </row>
     <row r="38" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
-      <c r="B38" s="52">
+      <c r="B38" s="62">
         <v>7</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="76"/>
-      <c r="H38" s="76"/>
-      <c r="I38" s="76"/>
-      <c r="J38" s="76"/>
-      <c r="K38" s="76"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="76"/>
-      <c r="N38" s="77"/>
-      <c r="O38" s="31"/>
-      <c r="P38" s="39"/>
-      <c r="Q38" s="40"/>
+      <c r="C38" s="63"/>
+      <c r="D38" s="76"/>
+      <c r="E38" s="77"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="49"/>
+      <c r="M38" s="49"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="105"/>
+      <c r="P38" s="93"/>
+      <c r="Q38" s="94"/>
       <c r="R38" s="1"/>
       <c r="AE38"/>
       <c r="AF38"/>
     </row>
     <row r="39" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
-      <c r="B39" s="53"/>
-      <c r="C39" s="56"/>
-      <c r="D39" s="34"/>
-      <c r="E39" s="35"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="76"/>
-      <c r="H39" s="76"/>
-      <c r="I39" s="76"/>
-      <c r="J39" s="76"/>
-      <c r="K39" s="76"/>
-      <c r="L39" s="76"/>
-      <c r="M39" s="76"/>
-      <c r="N39" s="77"/>
-      <c r="O39" s="31"/>
-      <c r="P39" s="39"/>
-      <c r="Q39" s="40"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="58"/>
+      <c r="D39" s="72"/>
+      <c r="E39" s="73"/>
+      <c r="F39" s="48"/>
+      <c r="G39" s="49"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="49"/>
+      <c r="M39" s="49"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="105"/>
+      <c r="P39" s="93"/>
+      <c r="Q39" s="94"/>
       <c r="R39" s="1"/>
       <c r="AE39"/>
       <c r="AF39"/>
     </row>
     <row r="40" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="57"/>
-      <c r="D40" s="36"/>
-      <c r="E40" s="37"/>
-      <c r="F40" s="78"/>
-      <c r="G40" s="79"/>
-      <c r="H40" s="79"/>
-      <c r="I40" s="79"/>
-      <c r="J40" s="79"/>
-      <c r="K40" s="79"/>
-      <c r="L40" s="79"/>
-      <c r="M40" s="79"/>
-      <c r="N40" s="80"/>
-      <c r="O40" s="31"/>
-      <c r="P40" s="39"/>
-      <c r="Q40" s="40"/>
+      <c r="B40" s="57"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="74"/>
+      <c r="E40" s="75"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="52"/>
+      <c r="M40" s="52"/>
+      <c r="N40" s="53"/>
+      <c r="O40" s="105"/>
+      <c r="P40" s="93"/>
+      <c r="Q40" s="94"/>
       <c r="R40" s="1"/>
       <c r="AE40"/>
       <c r="AF40"/>
     </row>
     <row r="41" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
-      <c r="B41" s="52">
+      <c r="B41" s="62">
         <v>8</v>
       </c>
-      <c r="C41" s="55"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="76"/>
-      <c r="H41" s="76"/>
-      <c r="I41" s="76"/>
-      <c r="J41" s="76"/>
-      <c r="K41" s="76"/>
-      <c r="L41" s="76"/>
-      <c r="M41" s="76"/>
-      <c r="N41" s="77"/>
-      <c r="O41" s="89"/>
-      <c r="P41" s="39"/>
-      <c r="Q41" s="40"/>
+      <c r="C41" s="63"/>
+      <c r="D41" s="76"/>
+      <c r="E41" s="77"/>
+      <c r="F41" s="48"/>
+      <c r="G41" s="49"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="49"/>
+      <c r="M41" s="49"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="102"/>
+      <c r="P41" s="93"/>
+      <c r="Q41" s="94"/>
       <c r="R41" s="1"/>
       <c r="AE41"/>
       <c r="AF41"/>
     </row>
     <row r="42" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="56"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="35"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="76"/>
-      <c r="H42" s="76"/>
-      <c r="I42" s="76"/>
-      <c r="J42" s="76"/>
-      <c r="K42" s="76"/>
-      <c r="L42" s="76"/>
-      <c r="M42" s="76"/>
-      <c r="N42" s="77"/>
-      <c r="O42" s="89"/>
-      <c r="P42" s="39"/>
-      <c r="Q42" s="40"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="58"/>
+      <c r="D42" s="72"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="48"/>
+      <c r="G42" s="49"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="49"/>
+      <c r="M42" s="49"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="102"/>
+      <c r="P42" s="93"/>
+      <c r="Q42" s="94"/>
       <c r="R42" s="1"/>
       <c r="AE42"/>
       <c r="AF42"/>
     </row>
     <row r="43" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
-      <c r="B43" s="54"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="36"/>
-      <c r="E43" s="37"/>
-      <c r="F43" s="78"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
-      <c r="J43" s="79"/>
-      <c r="K43" s="79"/>
-      <c r="L43" s="79"/>
-      <c r="M43" s="79"/>
-      <c r="N43" s="80"/>
-      <c r="O43" s="90"/>
-      <c r="P43" s="39"/>
-      <c r="Q43" s="40"/>
+      <c r="B43" s="57"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="74"/>
+      <c r="E43" s="75"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="52"/>
+      <c r="H43" s="52"/>
+      <c r="I43" s="52"/>
+      <c r="J43" s="52"/>
+      <c r="K43" s="52"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="52"/>
+      <c r="N43" s="53"/>
+      <c r="O43" s="103"/>
+      <c r="P43" s="93"/>
+      <c r="Q43" s="94"/>
       <c r="R43" s="1"/>
       <c r="AE43"/>
       <c r="AF43"/>
@@ -2885,20 +2886,20 @@
         <v>39</v>
       </c>
       <c r="C45"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="41"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="41"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="41"/>
-      <c r="O45" s="41"/>
-      <c r="P45" s="41"/>
-      <c r="Q45" s="41"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+      <c r="F45" s="54"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="54"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="54"/>
+      <c r="K45" s="54"/>
+      <c r="L45" s="54"/>
+      <c r="M45" s="54"/>
+      <c r="N45" s="54"/>
+      <c r="O45" s="54"/>
+      <c r="P45" s="54"/>
+      <c r="Q45" s="54"/>
       <c r="R45" s="6"/>
       <c r="AE45"/>
       <c r="AF45"/>
@@ -2907,20 +2908,20 @@
       <c r="A46" s="1"/>
       <c r="B46" s="6"/>
       <c r="C46"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="38"/>
-      <c r="F46" s="38"/>
-      <c r="G46" s="38"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="38"/>
-      <c r="L46" s="38"/>
-      <c r="M46" s="38"/>
-      <c r="N46" s="38"/>
-      <c r="O46" s="38"/>
-      <c r="P46" s="38"/>
-      <c r="Q46" s="38"/>
+      <c r="D46" s="55"/>
+      <c r="E46" s="55"/>
+      <c r="F46" s="55"/>
+      <c r="G46" s="55"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="55"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="55"/>
+      <c r="L46" s="55"/>
+      <c r="M46" s="55"/>
+      <c r="N46" s="55"/>
+      <c r="O46" s="55"/>
+      <c r="P46" s="55"/>
+      <c r="Q46" s="55"/>
       <c r="R46" s="6"/>
       <c r="AE46"/>
       <c r="AF46"/>
@@ -2929,20 +2930,20 @@
       <c r="A47" s="1"/>
       <c r="B47" s="6"/>
       <c r="C47"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="38"/>
-      <c r="G47" s="38"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="38"/>
-      <c r="J47" s="38"/>
-      <c r="K47" s="38"/>
-      <c r="L47" s="38"/>
-      <c r="M47" s="38"/>
-      <c r="N47" s="38"/>
-      <c r="O47" s="38"/>
-      <c r="P47" s="38"/>
-      <c r="Q47" s="38"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="55"/>
+      <c r="F47" s="55"/>
+      <c r="G47" s="55"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="55"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="55"/>
+      <c r="M47" s="55"/>
+      <c r="N47" s="55"/>
+      <c r="O47" s="55"/>
+      <c r="P47" s="55"/>
+      <c r="Q47" s="55"/>
       <c r="R47" s="6"/>
       <c r="AE47"/>
       <c r="AF47"/>
@@ -3017,62 +3018,62 @@
     </row>
     <row r="51" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
-      <c r="B51" s="28" t="s">
+      <c r="B51" s="60" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="D51" s="66" t="s">
+      <c r="D51" s="78" t="s">
         <v>18</v>
       </c>
-      <c r="E51" s="67"/>
-      <c r="F51" s="67"/>
-      <c r="G51" s="67"/>
-      <c r="H51" s="67"/>
-      <c r="I51" s="67"/>
-      <c r="J51" s="67"/>
-      <c r="K51" s="67"/>
-      <c r="L51" s="67"/>
-      <c r="M51" s="67"/>
-      <c r="N51" s="67"/>
-      <c r="O51" s="67"/>
-      <c r="P51" s="42" t="s">
+      <c r="E51" s="79"/>
+      <c r="F51" s="79"/>
+      <c r="G51" s="79"/>
+      <c r="H51" s="79"/>
+      <c r="I51" s="79"/>
+      <c r="J51" s="79"/>
+      <c r="K51" s="79"/>
+      <c r="L51" s="79"/>
+      <c r="M51" s="79"/>
+      <c r="N51" s="79"/>
+      <c r="O51" s="79"/>
+      <c r="P51" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="Q51" s="43"/>
+      <c r="Q51" s="88"/>
       <c r="R51" s="1"/>
       <c r="AE51"/>
       <c r="AF51"/>
     </row>
     <row r="52" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
-      <c r="B52" s="29"/>
-      <c r="C52" s="29"/>
-      <c r="D52" s="69"/>
-      <c r="E52" s="70"/>
-      <c r="F52" s="70"/>
-      <c r="G52" s="70"/>
-      <c r="H52" s="70"/>
-      <c r="I52" s="70"/>
-      <c r="J52" s="70"/>
-      <c r="K52" s="70"/>
-      <c r="L52" s="70"/>
-      <c r="M52" s="70"/>
-      <c r="N52" s="70"/>
-      <c r="O52" s="70"/>
-      <c r="P52" s="44"/>
-      <c r="Q52" s="45"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="81"/>
+      <c r="E52" s="82"/>
+      <c r="F52" s="82"/>
+      <c r="G52" s="82"/>
+      <c r="H52" s="82"/>
+      <c r="I52" s="82"/>
+      <c r="J52" s="82"/>
+      <c r="K52" s="82"/>
+      <c r="L52" s="82"/>
+      <c r="M52" s="82"/>
+      <c r="N52" s="82"/>
+      <c r="O52" s="82"/>
+      <c r="P52" s="89"/>
+      <c r="Q52" s="90"/>
       <c r="R52" s="1"/>
       <c r="AE52"/>
       <c r="AF52"/>
     </row>
     <row r="53" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
-      <c r="B53" s="53" t="s">
+      <c r="B53" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="C53" s="56"/>
+      <c r="C53" s="58"/>
       <c r="D53" s="23"/>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
@@ -3085,14 +3086,14 @@
       <c r="M53" s="24"/>
       <c r="N53" s="24"/>
       <c r="O53" s="24"/>
-      <c r="P53" s="46"/>
-      <c r="Q53" s="47"/>
+      <c r="P53" s="98"/>
+      <c r="Q53" s="99"/>
       <c r="R53" s="1"/>
     </row>
     <row r="54" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1"/>
-      <c r="B54" s="53"/>
-      <c r="C54" s="56"/>
+      <c r="B54" s="56"/>
+      <c r="C54" s="58"/>
       <c r="D54" s="26"/>
       <c r="E54" s="27"/>
       <c r="F54" s="27"/>
@@ -3105,14 +3106,14 @@
       <c r="M54" s="27"/>
       <c r="N54" s="27"/>
       <c r="O54" s="27"/>
-      <c r="P54" s="48"/>
-      <c r="Q54" s="49"/>
+      <c r="P54" s="100"/>
+      <c r="Q54" s="101"/>
       <c r="R54" s="1"/>
     </row>
     <row r="55" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1"/>
-      <c r="B55" s="54"/>
-      <c r="C55" s="57"/>
+      <c r="B55" s="57"/>
+      <c r="C55" s="59"/>
       <c r="D55" s="25"/>
       <c r="E55" s="22"/>
       <c r="F55" s="22"/>
@@ -3125,16 +3126,16 @@
       <c r="M55" s="22"/>
       <c r="N55" s="22"/>
       <c r="O55" s="22"/>
-      <c r="P55" s="48"/>
-      <c r="Q55" s="49"/>
+      <c r="P55" s="100"/>
+      <c r="Q55" s="101"/>
       <c r="R55" s="1"/>
     </row>
     <row r="56" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1"/>
-      <c r="B56" s="52" t="s">
+      <c r="B56" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="C56" s="55"/>
+      <c r="C56" s="63"/>
       <c r="D56" s="26"/>
       <c r="E56" s="27"/>
       <c r="F56" s="27"/>
@@ -3147,14 +3148,14 @@
       <c r="M56" s="27"/>
       <c r="N56" s="27"/>
       <c r="O56" s="27"/>
-      <c r="P56" s="48"/>
-      <c r="Q56" s="49"/>
+      <c r="P56" s="100"/>
+      <c r="Q56" s="101"/>
       <c r="R56" s="1"/>
     </row>
     <row r="57" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1"/>
-      <c r="B57" s="53"/>
-      <c r="C57" s="56"/>
+      <c r="B57" s="56"/>
+      <c r="C57" s="58"/>
       <c r="D57" s="26"/>
       <c r="E57" s="27"/>
       <c r="F57" s="27"/>
@@ -3167,14 +3168,14 @@
       <c r="M57" s="27"/>
       <c r="N57" s="27"/>
       <c r="O57" s="27"/>
-      <c r="P57" s="48"/>
-      <c r="Q57" s="49"/>
+      <c r="P57" s="100"/>
+      <c r="Q57" s="101"/>
       <c r="R57" s="1"/>
     </row>
     <row r="58" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1"/>
-      <c r="B58" s="54"/>
-      <c r="C58" s="57"/>
+      <c r="B58" s="57"/>
+      <c r="C58" s="59"/>
       <c r="D58" s="25"/>
       <c r="E58" s="22"/>
       <c r="F58" s="22"/>
@@ -3187,8 +3188,8 @@
       <c r="M58" s="22"/>
       <c r="N58" s="22"/>
       <c r="O58" s="22"/>
-      <c r="P58" s="48"/>
-      <c r="Q58" s="49"/>
+      <c r="P58" s="100"/>
+      <c r="Q58" s="101"/>
       <c r="R58" s="1"/>
     </row>
     <row r="59" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -3217,40 +3218,40 @@
         <v>38</v>
       </c>
       <c r="C60"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
-      <c r="F60" s="41"/>
-      <c r="G60" s="41"/>
-      <c r="H60" s="41"/>
-      <c r="I60" s="41"/>
-      <c r="J60" s="41"/>
-      <c r="K60" s="41"/>
-      <c r="L60" s="41"/>
-      <c r="M60" s="41"/>
-      <c r="N60" s="41"/>
-      <c r="O60" s="41"/>
-      <c r="P60" s="41"/>
-      <c r="Q60" s="41"/>
+      <c r="D60" s="54"/>
+      <c r="E60" s="54"/>
+      <c r="F60" s="54"/>
+      <c r="G60" s="54"/>
+      <c r="H60" s="54"/>
+      <c r="I60" s="54"/>
+      <c r="J60" s="54"/>
+      <c r="K60" s="54"/>
+      <c r="L60" s="54"/>
+      <c r="M60" s="54"/>
+      <c r="N60" s="54"/>
+      <c r="O60" s="54"/>
+      <c r="P60" s="54"/>
+      <c r="Q60" s="54"/>
       <c r="R60" s="6"/>
     </row>
     <row r="61" spans="1:32" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="6"/>
       <c r="C61"/>
-      <c r="D61" s="38"/>
-      <c r="E61" s="38"/>
-      <c r="F61" s="38"/>
-      <c r="G61" s="38"/>
-      <c r="H61" s="38"/>
-      <c r="I61" s="38"/>
-      <c r="J61" s="38"/>
-      <c r="K61" s="38"/>
-      <c r="L61" s="38"/>
-      <c r="M61" s="38"/>
-      <c r="N61" s="38"/>
-      <c r="O61" s="38"/>
-      <c r="P61" s="38"/>
-      <c r="Q61" s="38"/>
+      <c r="D61" s="55"/>
+      <c r="E61" s="55"/>
+      <c r="F61" s="55"/>
+      <c r="G61" s="55"/>
+      <c r="H61" s="55"/>
+      <c r="I61" s="55"/>
+      <c r="J61" s="55"/>
+      <c r="K61" s="55"/>
+      <c r="L61" s="55"/>
+      <c r="M61" s="55"/>
+      <c r="N61" s="55"/>
+      <c r="O61" s="55"/>
+      <c r="P61" s="55"/>
+      <c r="Q61" s="55"/>
       <c r="R61" s="6"/>
     </row>
     <row r="62" spans="1:32" ht="7.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -3396,21 +3397,21 @@
       <c r="B67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C67" s="50"/>
-      <c r="D67" s="50"/>
-      <c r="E67" s="50"/>
-      <c r="F67" s="50"/>
-      <c r="G67" s="50"/>
-      <c r="H67" s="50"/>
-      <c r="I67" s="50"/>
-      <c r="J67" s="50"/>
-      <c r="K67" s="50"/>
-      <c r="L67" s="50"/>
-      <c r="M67" s="50"/>
-      <c r="N67" s="50"/>
-      <c r="O67" s="50"/>
-      <c r="P67" s="50"/>
-      <c r="Q67" s="50"/>
+      <c r="C67" s="96"/>
+      <c r="D67" s="96"/>
+      <c r="E67" s="96"/>
+      <c r="F67" s="96"/>
+      <c r="G67" s="96"/>
+      <c r="H67" s="96"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="96"/>
+      <c r="K67" s="96"/>
+      <c r="L67" s="96"/>
+      <c r="M67" s="96"/>
+      <c r="N67" s="96"/>
+      <c r="O67" s="96"/>
+      <c r="P67" s="96"/>
+      <c r="Q67" s="96"/>
       <c r="R67" s="6"/>
       <c r="S67" s="14"/>
       <c r="T67" s="14"/>
@@ -3424,21 +3425,21 @@
     <row r="68" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="51"/>
-      <c r="E68" s="51"/>
-      <c r="F68" s="51"/>
-      <c r="G68" s="51"/>
-      <c r="H68" s="51"/>
-      <c r="I68" s="51"/>
-      <c r="J68" s="51"/>
-      <c r="K68" s="51"/>
-      <c r="L68" s="51"/>
-      <c r="M68" s="51"/>
-      <c r="N68" s="51"/>
-      <c r="O68" s="51"/>
-      <c r="P68" s="51"/>
-      <c r="Q68" s="51"/>
+      <c r="C68" s="97"/>
+      <c r="D68" s="97"/>
+      <c r="E68" s="97"/>
+      <c r="F68" s="97"/>
+      <c r="G68" s="97"/>
+      <c r="H68" s="97"/>
+      <c r="I68" s="97"/>
+      <c r="J68" s="97"/>
+      <c r="K68" s="97"/>
+      <c r="L68" s="97"/>
+      <c r="M68" s="97"/>
+      <c r="N68" s="97"/>
+      <c r="O68" s="97"/>
+      <c r="P68" s="97"/>
+      <c r="Q68" s="97"/>
       <c r="R68" s="6"/>
       <c r="S68" s="14"/>
       <c r="T68" s="14"/>
@@ -3570,21 +3571,21 @@
       <c r="B73" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C73" s="50"/>
-      <c r="D73" s="50"/>
-      <c r="E73" s="50"/>
-      <c r="F73" s="50"/>
-      <c r="G73" s="50"/>
-      <c r="H73" s="50"/>
-      <c r="I73" s="50"/>
-      <c r="J73" s="50"/>
-      <c r="K73" s="50"/>
-      <c r="L73" s="50"/>
-      <c r="M73" s="50"/>
-      <c r="N73" s="50"/>
-      <c r="O73" s="50"/>
-      <c r="P73" s="50"/>
-      <c r="Q73" s="50"/>
+      <c r="C73" s="96"/>
+      <c r="D73" s="96"/>
+      <c r="E73" s="96"/>
+      <c r="F73" s="96"/>
+      <c r="G73" s="96"/>
+      <c r="H73" s="96"/>
+      <c r="I73" s="96"/>
+      <c r="J73" s="96"/>
+      <c r="K73" s="96"/>
+      <c r="L73" s="96"/>
+      <c r="M73" s="96"/>
+      <c r="N73" s="96"/>
+      <c r="O73" s="96"/>
+      <c r="P73" s="96"/>
+      <c r="Q73" s="96"/>
       <c r="R73" s="6"/>
       <c r="S73" s="14"/>
       <c r="T73" s="14"/>
@@ -3598,21 +3599,21 @@
     <row r="74" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="51"/>
-      <c r="E74" s="51"/>
-      <c r="F74" s="51"/>
-      <c r="G74" s="51"/>
-      <c r="H74" s="51"/>
-      <c r="I74" s="51"/>
-      <c r="J74" s="51"/>
-      <c r="K74" s="51"/>
-      <c r="L74" s="51"/>
-      <c r="M74" s="51"/>
-      <c r="N74" s="51"/>
-      <c r="O74" s="51"/>
-      <c r="P74" s="51"/>
-      <c r="Q74" s="51"/>
+      <c r="C74" s="97"/>
+      <c r="D74" s="97"/>
+      <c r="E74" s="97"/>
+      <c r="F74" s="97"/>
+      <c r="G74" s="97"/>
+      <c r="H74" s="97"/>
+      <c r="I74" s="97"/>
+      <c r="J74" s="97"/>
+      <c r="K74" s="97"/>
+      <c r="L74" s="97"/>
+      <c r="M74" s="97"/>
+      <c r="N74" s="97"/>
+      <c r="O74" s="97"/>
+      <c r="P74" s="97"/>
+      <c r="Q74" s="97"/>
       <c r="R74" s="6"/>
       <c r="S74" s="14"/>
       <c r="T74" s="14"/>
@@ -3744,21 +3745,21 @@
       <c r="B79" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C79" s="50"/>
-      <c r="D79" s="50"/>
-      <c r="E79" s="50"/>
-      <c r="F79" s="50"/>
-      <c r="G79" s="50"/>
-      <c r="H79" s="50"/>
-      <c r="I79" s="50"/>
-      <c r="J79" s="50"/>
-      <c r="K79" s="50"/>
-      <c r="L79" s="50"/>
-      <c r="M79" s="50"/>
-      <c r="N79" s="50"/>
-      <c r="O79" s="50"/>
-      <c r="P79" s="50"/>
-      <c r="Q79" s="50"/>
+      <c r="C79" s="96"/>
+      <c r="D79" s="96"/>
+      <c r="E79" s="96"/>
+      <c r="F79" s="96"/>
+      <c r="G79" s="96"/>
+      <c r="H79" s="96"/>
+      <c r="I79" s="96"/>
+      <c r="J79" s="96"/>
+      <c r="K79" s="96"/>
+      <c r="L79" s="96"/>
+      <c r="M79" s="96"/>
+      <c r="N79" s="96"/>
+      <c r="O79" s="96"/>
+      <c r="P79" s="96"/>
+      <c r="Q79" s="96"/>
       <c r="R79" s="6"/>
       <c r="S79" s="14"/>
       <c r="T79" s="14"/>
@@ -3772,21 +3773,21 @@
     <row r="80" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="51"/>
-      <c r="D80" s="51"/>
-      <c r="E80" s="51"/>
-      <c r="F80" s="51"/>
-      <c r="G80" s="51"/>
-      <c r="H80" s="51"/>
-      <c r="I80" s="51"/>
-      <c r="J80" s="51"/>
-      <c r="K80" s="51"/>
-      <c r="L80" s="51"/>
-      <c r="M80" s="51"/>
-      <c r="N80" s="51"/>
-      <c r="O80" s="51"/>
-      <c r="P80" s="51"/>
-      <c r="Q80" s="51"/>
+      <c r="C80" s="97"/>
+      <c r="D80" s="97"/>
+      <c r="E80" s="97"/>
+      <c r="F80" s="97"/>
+      <c r="G80" s="97"/>
+      <c r="H80" s="97"/>
+      <c r="I80" s="97"/>
+      <c r="J80" s="97"/>
+      <c r="K80" s="97"/>
+      <c r="L80" s="97"/>
+      <c r="M80" s="97"/>
+      <c r="N80" s="97"/>
+      <c r="O80" s="97"/>
+      <c r="P80" s="97"/>
+      <c r="Q80" s="97"/>
       <c r="R80" s="6"/>
       <c r="S80" s="14"/>
       <c r="T80" s="14"/>
@@ -3918,21 +3919,21 @@
       <c r="B85" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
-      <c r="E85" s="50"/>
-      <c r="F85" s="50"/>
-      <c r="G85" s="50"/>
-      <c r="H85" s="50"/>
-      <c r="I85" s="50"/>
-      <c r="J85" s="50"/>
-      <c r="K85" s="50"/>
-      <c r="L85" s="50"/>
-      <c r="M85" s="50"/>
-      <c r="N85" s="50"/>
-      <c r="O85" s="50"/>
-      <c r="P85" s="50"/>
-      <c r="Q85" s="50"/>
+      <c r="C85" s="96"/>
+      <c r="D85" s="96"/>
+      <c r="E85" s="96"/>
+      <c r="F85" s="96"/>
+      <c r="G85" s="96"/>
+      <c r="H85" s="96"/>
+      <c r="I85" s="96"/>
+      <c r="J85" s="96"/>
+      <c r="K85" s="96"/>
+      <c r="L85" s="96"/>
+      <c r="M85" s="96"/>
+      <c r="N85" s="96"/>
+      <c r="O85" s="96"/>
+      <c r="P85" s="96"/>
+      <c r="Q85" s="96"/>
       <c r="R85" s="6"/>
       <c r="S85" s="14"/>
       <c r="T85" s="14"/>
@@ -3946,21 +3947,21 @@
     <row r="86" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
-      <c r="C86" s="51"/>
-      <c r="D86" s="51"/>
-      <c r="E86" s="51"/>
-      <c r="F86" s="51"/>
-      <c r="G86" s="51"/>
-      <c r="H86" s="51"/>
-      <c r="I86" s="51"/>
-      <c r="J86" s="51"/>
-      <c r="K86" s="51"/>
-      <c r="L86" s="51"/>
-      <c r="M86" s="51"/>
-      <c r="N86" s="51"/>
-      <c r="O86" s="51"/>
-      <c r="P86" s="51"/>
-      <c r="Q86" s="51"/>
+      <c r="C86" s="97"/>
+      <c r="D86" s="97"/>
+      <c r="E86" s="97"/>
+      <c r="F86" s="97"/>
+      <c r="G86" s="97"/>
+      <c r="H86" s="97"/>
+      <c r="I86" s="97"/>
+      <c r="J86" s="97"/>
+      <c r="K86" s="97"/>
+      <c r="L86" s="97"/>
+      <c r="M86" s="97"/>
+      <c r="N86" s="97"/>
+      <c r="O86" s="97"/>
+      <c r="P86" s="97"/>
+      <c r="Q86" s="97"/>
       <c r="R86" s="6"/>
       <c r="S86" s="14"/>
       <c r="T86" s="14"/>
@@ -4092,21 +4093,21 @@
       <c r="B91" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
-      <c r="E91" s="50"/>
-      <c r="F91" s="50"/>
-      <c r="G91" s="50"/>
-      <c r="H91" s="50"/>
-      <c r="I91" s="50"/>
-      <c r="J91" s="50"/>
-      <c r="K91" s="50"/>
-      <c r="L91" s="50"/>
-      <c r="M91" s="50"/>
-      <c r="N91" s="50"/>
-      <c r="O91" s="50"/>
-      <c r="P91" s="50"/>
-      <c r="Q91" s="50"/>
+      <c r="C91" s="96"/>
+      <c r="D91" s="96"/>
+      <c r="E91" s="96"/>
+      <c r="F91" s="96"/>
+      <c r="G91" s="96"/>
+      <c r="H91" s="96"/>
+      <c r="I91" s="96"/>
+      <c r="J91" s="96"/>
+      <c r="K91" s="96"/>
+      <c r="L91" s="96"/>
+      <c r="M91" s="96"/>
+      <c r="N91" s="96"/>
+      <c r="O91" s="96"/>
+      <c r="P91" s="96"/>
+      <c r="Q91" s="96"/>
       <c r="R91" s="6"/>
       <c r="S91" s="14"/>
       <c r="T91" s="14"/>
@@ -4120,21 +4121,21 @@
     <row r="92" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
-      <c r="C92" s="51"/>
-      <c r="D92" s="51"/>
-      <c r="E92" s="51"/>
-      <c r="F92" s="51"/>
-      <c r="G92" s="51"/>
-      <c r="H92" s="51"/>
-      <c r="I92" s="51"/>
-      <c r="J92" s="51"/>
-      <c r="K92" s="51"/>
-      <c r="L92" s="51"/>
-      <c r="M92" s="51"/>
-      <c r="N92" s="51"/>
-      <c r="O92" s="51"/>
-      <c r="P92" s="51"/>
-      <c r="Q92" s="51"/>
+      <c r="C92" s="97"/>
+      <c r="D92" s="97"/>
+      <c r="E92" s="97"/>
+      <c r="F92" s="97"/>
+      <c r="G92" s="97"/>
+      <c r="H92" s="97"/>
+      <c r="I92" s="97"/>
+      <c r="J92" s="97"/>
+      <c r="K92" s="97"/>
+      <c r="L92" s="97"/>
+      <c r="M92" s="97"/>
+      <c r="N92" s="97"/>
+      <c r="O92" s="97"/>
+      <c r="P92" s="97"/>
+      <c r="Q92" s="97"/>
       <c r="R92" s="6"/>
       <c r="S92" s="14"/>
       <c r="T92" s="14"/>
@@ -4266,21 +4267,21 @@
       <c r="B97" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="50"/>
-      <c r="F97" s="50"/>
-      <c r="G97" s="50"/>
-      <c r="H97" s="50"/>
-      <c r="I97" s="50"/>
-      <c r="J97" s="50"/>
-      <c r="K97" s="50"/>
-      <c r="L97" s="50"/>
-      <c r="M97" s="50"/>
-      <c r="N97" s="50"/>
-      <c r="O97" s="50"/>
-      <c r="P97" s="50"/>
-      <c r="Q97" s="50"/>
+      <c r="C97" s="96"/>
+      <c r="D97" s="96"/>
+      <c r="E97" s="96"/>
+      <c r="F97" s="96"/>
+      <c r="G97" s="96"/>
+      <c r="H97" s="96"/>
+      <c r="I97" s="96"/>
+      <c r="J97" s="96"/>
+      <c r="K97" s="96"/>
+      <c r="L97" s="96"/>
+      <c r="M97" s="96"/>
+      <c r="N97" s="96"/>
+      <c r="O97" s="96"/>
+      <c r="P97" s="96"/>
+      <c r="Q97" s="96"/>
       <c r="R97" s="6"/>
       <c r="S97" s="14"/>
       <c r="T97" s="14"/>
@@ -4294,21 +4295,21 @@
     <row r="98" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
-      <c r="C98" s="51"/>
-      <c r="D98" s="51"/>
-      <c r="E98" s="51"/>
-      <c r="F98" s="51"/>
-      <c r="G98" s="51"/>
-      <c r="H98" s="51"/>
-      <c r="I98" s="51"/>
-      <c r="J98" s="51"/>
-      <c r="K98" s="51"/>
-      <c r="L98" s="51"/>
-      <c r="M98" s="51"/>
-      <c r="N98" s="51"/>
-      <c r="O98" s="51"/>
-      <c r="P98" s="51"/>
-      <c r="Q98" s="51"/>
+      <c r="C98" s="97"/>
+      <c r="D98" s="97"/>
+      <c r="E98" s="97"/>
+      <c r="F98" s="97"/>
+      <c r="G98" s="97"/>
+      <c r="H98" s="97"/>
+      <c r="I98" s="97"/>
+      <c r="J98" s="97"/>
+      <c r="K98" s="97"/>
+      <c r="L98" s="97"/>
+      <c r="M98" s="97"/>
+      <c r="N98" s="97"/>
+      <c r="O98" s="97"/>
+      <c r="P98" s="97"/>
+      <c r="Q98" s="97"/>
       <c r="R98" s="6"/>
       <c r="S98" s="14"/>
       <c r="T98" s="14"/>
@@ -4440,21 +4441,21 @@
       <c r="B103" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C103" s="50"/>
-      <c r="D103" s="50"/>
-      <c r="E103" s="50"/>
-      <c r="F103" s="50"/>
-      <c r="G103" s="50"/>
-      <c r="H103" s="50"/>
-      <c r="I103" s="50"/>
-      <c r="J103" s="50"/>
-      <c r="K103" s="50"/>
-      <c r="L103" s="50"/>
-      <c r="M103" s="50"/>
-      <c r="N103" s="50"/>
-      <c r="O103" s="50"/>
-      <c r="P103" s="50"/>
-      <c r="Q103" s="50"/>
+      <c r="C103" s="96"/>
+      <c r="D103" s="96"/>
+      <c r="E103" s="96"/>
+      <c r="F103" s="96"/>
+      <c r="G103" s="96"/>
+      <c r="H103" s="96"/>
+      <c r="I103" s="96"/>
+      <c r="J103" s="96"/>
+      <c r="K103" s="96"/>
+      <c r="L103" s="96"/>
+      <c r="M103" s="96"/>
+      <c r="N103" s="96"/>
+      <c r="O103" s="96"/>
+      <c r="P103" s="96"/>
+      <c r="Q103" s="96"/>
       <c r="R103" s="6"/>
       <c r="S103" s="14"/>
       <c r="T103" s="14"/>
@@ -4468,21 +4469,21 @@
     <row r="104" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1"/>
       <c r="B104" s="1"/>
-      <c r="C104" s="51"/>
-      <c r="D104" s="51"/>
-      <c r="E104" s="51"/>
-      <c r="F104" s="51"/>
-      <c r="G104" s="51"/>
-      <c r="H104" s="51"/>
-      <c r="I104" s="51"/>
-      <c r="J104" s="51"/>
-      <c r="K104" s="51"/>
-      <c r="L104" s="51"/>
-      <c r="M104" s="51"/>
-      <c r="N104" s="51"/>
-      <c r="O104" s="51"/>
-      <c r="P104" s="51"/>
-      <c r="Q104" s="51"/>
+      <c r="C104" s="97"/>
+      <c r="D104" s="97"/>
+      <c r="E104" s="97"/>
+      <c r="F104" s="97"/>
+      <c r="G104" s="97"/>
+      <c r="H104" s="97"/>
+      <c r="I104" s="97"/>
+      <c r="J104" s="97"/>
+      <c r="K104" s="97"/>
+      <c r="L104" s="97"/>
+      <c r="M104" s="97"/>
+      <c r="N104" s="97"/>
+      <c r="O104" s="97"/>
+      <c r="P104" s="97"/>
+      <c r="Q104" s="97"/>
       <c r="R104" s="6"/>
       <c r="S104" s="14"/>
       <c r="T104" s="14"/>
@@ -4614,21 +4615,21 @@
       <c r="B109" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C109" s="50"/>
-      <c r="D109" s="50"/>
-      <c r="E109" s="50"/>
-      <c r="F109" s="50"/>
-      <c r="G109" s="50"/>
-      <c r="H109" s="50"/>
-      <c r="I109" s="50"/>
-      <c r="J109" s="50"/>
-      <c r="K109" s="50"/>
-      <c r="L109" s="50"/>
-      <c r="M109" s="50"/>
-      <c r="N109" s="50"/>
-      <c r="O109" s="50"/>
-      <c r="P109" s="50"/>
-      <c r="Q109" s="50"/>
+      <c r="C109" s="96"/>
+      <c r="D109" s="96"/>
+      <c r="E109" s="96"/>
+      <c r="F109" s="96"/>
+      <c r="G109" s="96"/>
+      <c r="H109" s="96"/>
+      <c r="I109" s="96"/>
+      <c r="J109" s="96"/>
+      <c r="K109" s="96"/>
+      <c r="L109" s="96"/>
+      <c r="M109" s="96"/>
+      <c r="N109" s="96"/>
+      <c r="O109" s="96"/>
+      <c r="P109" s="96"/>
+      <c r="Q109" s="96"/>
       <c r="R109" s="6"/>
       <c r="S109" s="14"/>
       <c r="T109" s="14"/>
@@ -4642,21 +4643,21 @@
     <row r="110" spans="1:26" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1"/>
       <c r="B110" s="1"/>
-      <c r="C110" s="51"/>
-      <c r="D110" s="51"/>
-      <c r="E110" s="51"/>
-      <c r="F110" s="51"/>
-      <c r="G110" s="51"/>
-      <c r="H110" s="51"/>
-      <c r="I110" s="51"/>
-      <c r="J110" s="51"/>
-      <c r="K110" s="51"/>
-      <c r="L110" s="51"/>
-      <c r="M110" s="51"/>
-      <c r="N110" s="51"/>
-      <c r="O110" s="51"/>
-      <c r="P110" s="51"/>
-      <c r="Q110" s="51"/>
+      <c r="C110" s="97"/>
+      <c r="D110" s="97"/>
+      <c r="E110" s="97"/>
+      <c r="F110" s="97"/>
+      <c r="G110" s="97"/>
+      <c r="H110" s="97"/>
+      <c r="I110" s="97"/>
+      <c r="J110" s="97"/>
+      <c r="K110" s="97"/>
+      <c r="L110" s="97"/>
+      <c r="M110" s="97"/>
+      <c r="N110" s="97"/>
+      <c r="O110" s="97"/>
+      <c r="P110" s="97"/>
+      <c r="Q110" s="97"/>
       <c r="R110" s="6"/>
       <c r="S110" s="14"/>
       <c r="T110" s="14"/>
@@ -8967,81 +8968,18 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="113">
-    <mergeCell ref="N4:N5"/>
-    <mergeCell ref="O4:Q5"/>
-    <mergeCell ref="G4:L4"/>
-    <mergeCell ref="G5:L5"/>
-    <mergeCell ref="G6:L6"/>
-    <mergeCell ref="G7:L7"/>
-    <mergeCell ref="G8:L8"/>
-    <mergeCell ref="P13:Q14"/>
-    <mergeCell ref="N10:O11"/>
-    <mergeCell ref="P10:Q11"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="J11:L14"/>
-    <mergeCell ref="N7:O8"/>
-    <mergeCell ref="P7:Q8"/>
-    <mergeCell ref="F41:N41"/>
-    <mergeCell ref="F42:N43"/>
-    <mergeCell ref="D45:Q45"/>
-    <mergeCell ref="D46:Q46"/>
-    <mergeCell ref="D47:Q47"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B41:B43"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C35:C37"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="C56:C58"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="B38:B40"/>
-    <mergeCell ref="C38:C40"/>
-    <mergeCell ref="H1:L1"/>
-    <mergeCell ref="B2:P2"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="D18:E19"/>
-    <mergeCell ref="D20:E22"/>
-    <mergeCell ref="D23:E25"/>
-    <mergeCell ref="F18:N19"/>
-    <mergeCell ref="F20:N20"/>
-    <mergeCell ref="F21:N22"/>
-    <mergeCell ref="F23:N23"/>
-    <mergeCell ref="F24:N25"/>
-    <mergeCell ref="P18:Q19"/>
-    <mergeCell ref="P20:Q22"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="N13:O14"/>
-    <mergeCell ref="C109:Q109"/>
-    <mergeCell ref="C110:Q110"/>
-    <mergeCell ref="C97:Q97"/>
-    <mergeCell ref="C98:Q98"/>
-    <mergeCell ref="C103:Q103"/>
-    <mergeCell ref="C104:Q104"/>
-    <mergeCell ref="C67:Q67"/>
-    <mergeCell ref="C68:Q68"/>
-    <mergeCell ref="C85:Q85"/>
-    <mergeCell ref="C73:Q73"/>
-    <mergeCell ref="C74:Q74"/>
-    <mergeCell ref="C79:Q79"/>
-    <mergeCell ref="C80:Q80"/>
-    <mergeCell ref="C91:Q91"/>
-    <mergeCell ref="C92:Q92"/>
-    <mergeCell ref="C86:Q86"/>
+    <mergeCell ref="O23:O25"/>
+    <mergeCell ref="O26:O28"/>
+    <mergeCell ref="O29:O31"/>
+    <mergeCell ref="O32:O34"/>
+    <mergeCell ref="O35:O37"/>
+    <mergeCell ref="O38:O40"/>
+    <mergeCell ref="D32:E34"/>
+    <mergeCell ref="D35:E37"/>
+    <mergeCell ref="F35:N35"/>
+    <mergeCell ref="F36:N37"/>
+    <mergeCell ref="F38:N38"/>
+    <mergeCell ref="F39:N40"/>
     <mergeCell ref="D61:Q61"/>
     <mergeCell ref="P23:Q25"/>
     <mergeCell ref="P26:Q28"/>
@@ -9066,20 +9004,83 @@
     <mergeCell ref="O41:O43"/>
     <mergeCell ref="F32:N32"/>
     <mergeCell ref="F33:N34"/>
+    <mergeCell ref="C109:Q109"/>
+    <mergeCell ref="C110:Q110"/>
+    <mergeCell ref="C97:Q97"/>
+    <mergeCell ref="C98:Q98"/>
+    <mergeCell ref="C103:Q103"/>
+    <mergeCell ref="C104:Q104"/>
+    <mergeCell ref="C67:Q67"/>
+    <mergeCell ref="C68:Q68"/>
+    <mergeCell ref="C85:Q85"/>
+    <mergeCell ref="C73:Q73"/>
+    <mergeCell ref="C74:Q74"/>
+    <mergeCell ref="C79:Q79"/>
+    <mergeCell ref="C80:Q80"/>
+    <mergeCell ref="C91:Q91"/>
+    <mergeCell ref="C92:Q92"/>
+    <mergeCell ref="C86:Q86"/>
+    <mergeCell ref="H1:L1"/>
+    <mergeCell ref="B2:P2"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="D18:E19"/>
+    <mergeCell ref="D20:E22"/>
+    <mergeCell ref="D23:E25"/>
+    <mergeCell ref="F18:N19"/>
+    <mergeCell ref="F20:N20"/>
+    <mergeCell ref="F21:N22"/>
+    <mergeCell ref="F23:N23"/>
+    <mergeCell ref="F24:N25"/>
+    <mergeCell ref="P18:Q19"/>
+    <mergeCell ref="P20:Q22"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="N13:O14"/>
     <mergeCell ref="O18:O19"/>
     <mergeCell ref="O20:O22"/>
-    <mergeCell ref="O23:O25"/>
-    <mergeCell ref="O26:O28"/>
-    <mergeCell ref="O29:O31"/>
-    <mergeCell ref="O32:O34"/>
-    <mergeCell ref="O35:O37"/>
-    <mergeCell ref="O38:O40"/>
-    <mergeCell ref="D32:E34"/>
-    <mergeCell ref="D35:E37"/>
-    <mergeCell ref="F35:N35"/>
-    <mergeCell ref="F36:N37"/>
-    <mergeCell ref="F38:N38"/>
-    <mergeCell ref="F39:N40"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C35:C37"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="C29:C31"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="C56:C58"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="F41:N41"/>
+    <mergeCell ref="F42:N43"/>
+    <mergeCell ref="D45:Q45"/>
+    <mergeCell ref="D46:Q46"/>
+    <mergeCell ref="D47:Q47"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="N4:N5"/>
+    <mergeCell ref="O4:Q5"/>
+    <mergeCell ref="G4:L4"/>
+    <mergeCell ref="G5:L5"/>
+    <mergeCell ref="G6:L6"/>
+    <mergeCell ref="G7:L7"/>
+    <mergeCell ref="G8:L8"/>
+    <mergeCell ref="P13:Q14"/>
+    <mergeCell ref="N10:O11"/>
+    <mergeCell ref="P10:Q11"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J11:L14"/>
+    <mergeCell ref="N7:O8"/>
+    <mergeCell ref="P7:Q8"/>
   </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -9167,6 +9168,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A2B826667128664EB5BF996137814269" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fae99688d4eff97766fcbf054e39ddba">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="cef818d1-7f02-40bd-b635-f979fe7dc7c8" xmlns:ns3="123f82ff-efc3-4fb3-befe-02b68418169f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d2063e240d92a77e1e922105c74daf1d" ns2:_="" ns3:_="">
     <xsd:import namespace="cef818d1-7f02-40bd-b635-f979fe7dc7c8"/>
@@ -9383,36 +9399,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0240A04-A3AB-4903-A7D7-B79D60CC1221}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57E74503-2AD6-4615-B95D-C25393FC43B6}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="cef818d1-7f02-40bd-b635-f979fe7dc7c8"/>
-    <ds:schemaRef ds:uri="123f82ff-efc3-4fb3-befe-02b68418169f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9435,9 +9425,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57E74503-2AD6-4615-B95D-C25393FC43B6}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0240A04-A3AB-4903-A7D7-B79D60CC1221}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="cef818d1-7f02-40bd-b635-f979fe7dc7c8"/>
+    <ds:schemaRef ds:uri="123f82ff-efc3-4fb3-befe-02b68418169f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>